<commit_message>
added stamp test case
</commit_message>
<xml_diff>
--- a/testcase/testcase.xlsx
+++ b/testcase/testcase.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="446">
   <si>
     <t>序号</t>
   </si>
@@ -8017,6 +8017,24 @@
     <t>TC2016</t>
   </si>
   <si>
+    <t>TC2017</t>
+  </si>
+  <si>
+    <t>TC2018</t>
+  </si>
+  <si>
+    <t>TC2019</t>
+  </si>
+  <si>
+    <t>TC2020</t>
+  </si>
+  <si>
+    <t>TC2021</t>
+  </si>
+  <si>
+    <t>TC2022</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -8042,25 +8060,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>时，少于</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>66</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>字节的</t>
+      <t>时，</t>
     </r>
     <r>
       <rPr>
@@ -8078,11 +8078,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>地址</t>
-    </r>
-  </si>
-  <si>
-    <t>TC2017</t>
+      <t>地址为字符串</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: 0x</t>
+    </r>
+  </si>
+  <si>
+    <t>TC2023</t>
   </si>
   <si>
     <r>
@@ -8110,25 +8119,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>时，多于</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>66</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>字节的</t>
+      <t>时，输入</t>
     </r>
     <r>
       <rPr>
@@ -8146,11 +8137,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>地址</t>
-    </r>
-  </si>
-  <si>
-    <t>TC2018</t>
+      <t>地址为十进制整数</t>
+    </r>
+  </si>
+  <si>
+    <t>TC2024</t>
+  </si>
+  <si>
+    <t>TC2025</t>
   </si>
   <si>
     <r>
@@ -8187,354 +8181,6 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>66</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>字节少一个字符的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>stamp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>地址</t>
-    </r>
-  </si>
-  <si>
-    <t>TC2019</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>创建</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>时，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>stamp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>地址不带</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>0x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>前缀</t>
-    </r>
-  </si>
-  <si>
-    <t>TC2020</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>创建</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>时，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>stamp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>地址为无效十六进制（比如包含非十六进制字符）</t>
-    </r>
-  </si>
-  <si>
-    <t>TC2021</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>创建</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>时，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>stamp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>地址为空字符串</t>
-    </r>
-  </si>
-  <si>
-    <t>TC2022</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>创建</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>时，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>stamp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>地址为字符串</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>: 0x</t>
-    </r>
-  </si>
-  <si>
-    <t>TC2023</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>创建</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>时，输入</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>stamp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>地址为十进制整数</t>
-    </r>
-  </si>
-  <si>
-    <t>TC2024</t>
-  </si>
-  <si>
-    <t>TC2025</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>创建</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>时，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t>value</t>
     </r>
     <r>
@@ -8627,30 +8273,6 @@
   </si>
   <si>
     <t>from地址长度不够，多一个byte</t>
-  </si>
-  <si>
-    <r>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>为</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>-0.01</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>无效的value</t>
@@ -8672,6 +8294,126 @@
   </si>
   <si>
     <t>test case</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>value为-0.01</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>value为0</t>
+  </si>
+  <si>
+    <t>value为-0</t>
+  </si>
+  <si>
+    <t>无效的data</t>
+  </si>
+  <si>
+    <t>创建data时，少于66字节的stamp地址</t>
+  </si>
+  <si>
+    <t>提示无效的OTA地址</t>
+  </si>
+  <si>
+    <t>创建data时，多于66字节的stamp地址</t>
+  </si>
+  <si>
+    <t>创建data时，66字节少一个字符的stamp地址</t>
+  </si>
+  <si>
+    <t>创建data时，stamp地址不带0x前缀</t>
+  </si>
+  <si>
+    <t>提示缺少0x前缀</t>
+  </si>
+  <si>
+    <t>创建data时，stamp地址为无效十六进制（比如包含非十六进制字符）</t>
+  </si>
+  <si>
+    <t>创建data时，stamp地址为空字符串</t>
+  </si>
+  <si>
+    <r>
+      <t>创建</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>时，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>填写</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000wancoin</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>gasprice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>设置为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>-20000000000</t>
+    </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -8788,7 +8530,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -8824,6 +8566,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -8834,7 +8587,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -8888,6 +8641,12 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -11231,21 +10990,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44:I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.77734375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="16384" width="13.77734375" style="31"/>
+    <col min="1" max="3" width="13.77734375" style="31"/>
+    <col min="4" max="4" width="43.21875" style="31" customWidth="1"/>
+    <col min="5" max="16384" width="13.77734375" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4">
       <c r="A1" s="31" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1">
@@ -11256,19 +11017,19 @@
         <v>379</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
       <c r="G2" s="27" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="H2" s="27"/>
       <c r="I2" s="30" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="J2" s="29"/>
       <c r="K2" s="25"/>
@@ -11280,48 +11041,48 @@
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="14.4">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="43.2">
       <c r="A4" s="27" t="s">
         <v>381</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
       <c r="D4" s="28" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
       <c r="I4" s="27" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="14.4">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="43.2">
       <c r="A5" s="27" t="s">
         <v>382</v>
       </c>
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
       <c r="D5" s="28" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
       <c r="I5" s="27" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.4">
@@ -11341,213 +11102,306 @@
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="27" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="27" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="14.4">
+      <c r="A8" s="30" t="s">
+        <v>384</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35" t="s">
+        <v>432</v>
+      </c>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34" t="s">
+        <v>425</v>
+      </c>
+      <c r="H8" s="34"/>
+      <c r="I8" s="33" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="34" customFormat="1" ht="14.4">
+      <c r="A9" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>433</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>425</v>
+      </c>
+      <c r="I9" s="33" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="14.4">
+      <c r="A10" s="30" t="s">
+        <v>386</v>
+      </c>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="35" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="13.2">
-      <c r="A8" s="32" t="s">
-        <v>384</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34" t="s">
+        <v>425</v>
+      </c>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34" t="s">
         <v>430</v>
       </c>
-      <c r="G8" s="31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="13.2">
-      <c r="A9" s="32" t="s">
-        <v>385</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="13.2">
-      <c r="A10" s="32" t="s">
-        <v>386</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="13.2">
-      <c r="A12" s="32" t="s">
+    </row>
+    <row r="12" spans="1:11" ht="14.4">
+      <c r="A12" s="30" t="s">
         <v>387</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34" t="s">
+        <v>435</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>436</v>
+      </c>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
+        <v>437</v>
+      </c>
+      <c r="H12" s="34"/>
+      <c r="I12" s="36" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="14.4">
+      <c r="A13" s="30" t="s">
         <v>388</v>
       </c>
-      <c r="G12" s="31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="13.2">
-      <c r="A13" s="32" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35" t="s">
+        <v>438</v>
+      </c>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34" t="s">
+        <v>437</v>
+      </c>
+      <c r="H13" s="34"/>
+      <c r="I13" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="14.4">
+      <c r="A14" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="35" t="s">
+        <v>439</v>
+      </c>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34" t="s">
+        <v>437</v>
+      </c>
+      <c r="H14" s="34"/>
+      <c r="I14" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14.4">
+      <c r="A15" s="30" t="s">
         <v>390</v>
       </c>
-      <c r="G13" s="31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="13.2">
-      <c r="A14" s="32" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35" t="s">
+        <v>440</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34" t="s">
+        <v>441</v>
+      </c>
+      <c r="H15" s="34"/>
+      <c r="I15" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="28.8">
+      <c r="A16" s="30" t="s">
         <v>391</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34" t="s">
+        <v>437</v>
+      </c>
+      <c r="H16" s="34"/>
+      <c r="I16" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.4">
+      <c r="A17" s="30" t="s">
         <v>392</v>
       </c>
-      <c r="G14" s="31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="13.2">
-      <c r="A15" s="32" t="s">
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="35" t="s">
+        <v>443</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34" t="s">
+        <v>437</v>
+      </c>
+      <c r="H17" s="34"/>
+      <c r="I17" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.4">
+      <c r="A18" s="32" t="s">
         <v>393</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D18" s="9" t="s">
         <v>394</v>
-      </c>
-      <c r="G15" s="31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="26.4">
-      <c r="A16" s="32" t="s">
-        <v>395</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="G16" s="31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="13.2">
-      <c r="A17" s="32" t="s">
-        <v>397</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="13.2">
-      <c r="A18" s="32" t="s">
-        <v>399</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>400</v>
       </c>
       <c r="G18" s="31" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="13.2">
+      <c r="I18" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14.4">
       <c r="A19" s="32" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="G19" s="31" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="13.2">
+      <c r="I19" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="13.2">
       <c r="A20" s="32" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:7" ht="13.2">
+    <row r="21" spans="1:9" ht="14.4">
       <c r="A21" s="32" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="G21" s="31" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="13.2">
+      <c r="I21" s="36" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14.4">
       <c r="A22" s="32" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="13.2">
+      <c r="I22" s="36" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14.4">
       <c r="A23" s="32" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="39.6">
+      <c r="I23" s="36" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="52.8">
       <c r="A24" s="32" t="s">
-        <v>408</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="13.2">
+        <v>402</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="I24" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14.4">
       <c r="A25" s="32" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="13.2">
+      <c r="I25" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14.4">
       <c r="A26" s="32" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="13.2">
+      <c r="I26" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.4">
       <c r="A27" s="32" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="13.2">
+      <c r="I27" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14.4">
       <c r="A29" s="32" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>72</v>
@@ -11555,10 +11409,13 @@
       <c r="G29" s="31" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="13.2">
+      <c r="I29" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="14.4">
       <c r="A30" s="32" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>74</v>
@@ -11566,10 +11423,13 @@
       <c r="G30" s="31" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="13.2">
+      <c r="I30" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14.4">
       <c r="A31" s="32" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>77</v>
@@ -11577,10 +11437,13 @@
       <c r="G31" s="31" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="13.2">
+      <c r="I31" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14.4">
       <c r="A32" s="32" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>79</v>
@@ -11588,10 +11451,13 @@
       <c r="G32" s="31" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="13.2">
+      <c r="I32" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14.4">
       <c r="A33" s="32" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>81</v>
@@ -11599,10 +11465,13 @@
       <c r="G33" s="31" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="13.2">
+      <c r="I33" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="14.4">
       <c r="A34" s="32" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>83</v>
@@ -11610,10 +11479,18 @@
       <c r="G34" s="31" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="13.2">
+      <c r="I34" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="14.4">
+      <c r="I35" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="14.4">
       <c r="A36" s="32" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="C36" s="31" t="s">
         <v>85</v>
@@ -11624,10 +11501,13 @@
       <c r="G36" s="31" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="13.2">
+      <c r="I36" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="14.4">
       <c r="A37" s="32" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>89</v>
@@ -11635,10 +11515,13 @@
       <c r="G37" s="31" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="13.2">
+      <c r="I37" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="14.4">
       <c r="A38" s="32" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>92</v>
@@ -11646,10 +11529,13 @@
       <c r="G38" s="31" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="13.2">
+      <c r="I38" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="14.4">
       <c r="A40" s="32" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="C40" s="31" t="s">
         <v>94</v>
@@ -11660,27 +11546,36 @@
       <c r="G40" s="31" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="13.2">
+      <c r="I40" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="14.4">
       <c r="A41" s="32" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>98</v>
+        <v>445</v>
       </c>
       <c r="G41" s="31" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="13.2">
+      <c r="I41" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="14.4">
       <c r="A42" s="32" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>101</v>
       </c>
       <c r="G42" s="31" t="s">
         <v>99</v>
+      </c>
+      <c r="I42" s="36" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct some issues of test cases
</commit_message>
<xml_diff>
--- a/testcase/testcase.xlsx
+++ b/testcase/testcase.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="wancoin" sheetId="1" r:id="rId1"/>
     <sheet name="wantoken" sheetId="2" r:id="rId2"/>
     <sheet name="stamp" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="454">
   <si>
     <t>序号</t>
   </si>
@@ -779,71 +779,6 @@
         <charset val="1"/>
       </rPr>
       <t>data</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>创建</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>时，少于</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>66</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>字节的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>OTA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>地址</t>
     </r>
   </si>
   <si>
@@ -8413,6 +8348,223 @@
         <charset val="1"/>
       </rPr>
       <t>-20000000000</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>创建</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>时，少于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>66</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>字节的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>OTA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>地址</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>sendTransaction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>时，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>为包含非十六进制字符</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>gasprice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>设置为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>'0x0'</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC1059</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>输入伪造的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>OTA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>地址</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC1096</t>
+  </si>
+  <si>
+    <r>
+      <t>创建</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>时，只输入环签名，不输入value</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC1105</t>
+  </si>
+  <si>
+    <r>
+      <t>创建</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>时，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>填写空字符串</t>
     </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -8488,7 +8640,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8527,6 +8679,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -8587,7 +8745,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -8647,6 +8805,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -8734,7 +8897,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CEEACA"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -9011,21 +9174,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H126"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G101" sqref="G101"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="11.33203125"/>
-    <col min="2" max="2" width="21.109375"/>
-    <col min="3" max="3" width="24.5546875"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
     <col min="4" max="4" width="46" style="1"/>
     <col min="5" max="5" width="22"/>
     <col min="6" max="6" width="20"/>
-    <col min="7" max="7" width="58.21875"/>
+    <col min="7" max="7" width="39.88671875" customWidth="1"/>
     <col min="8" max="8" width="58.88671875"/>
   </cols>
   <sheetData>
@@ -9193,87 +9356,87 @@
         <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="G16" t="s">
         <v>38</v>
-      </c>
-      <c r="G16" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="13.2">
       <c r="A17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="13.2">
       <c r="A18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="13.2">
       <c r="A19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="G19" t="s">
         <v>45</v>
-      </c>
-      <c r="G19" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="26.4">
       <c r="A20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="G20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="13.2">
       <c r="A21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="G21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="13.2">
       <c r="A22" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="G22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="13.2">
       <c r="A23" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="G23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="13.2">
@@ -9281,64 +9444,67 @@
     </row>
     <row r="25" spans="1:8" ht="13.2">
       <c r="A25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="G25" t="s">
         <v>56</v>
-      </c>
-      <c r="G25" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="13.2">
       <c r="A26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="13.2">
       <c r="A27" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="52.8">
       <c r="A28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="13.2">
       <c r="A29" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="11" customFormat="1" ht="13.2">
       <c r="A30" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="H30" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H30" s="13" t="s">
+    </row>
+    <row r="31" spans="1:8" s="11" customFormat="1" ht="13.2">
+      <c r="A31" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="13.2">
-      <c r="A31" s="6" t="s">
+      <c r="D31" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>70</v>
+      <c r="H31" s="13" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -9346,68 +9512,68 @@
     </row>
     <row r="33" spans="1:7" ht="13.2">
       <c r="A33" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="G33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="13.2">
       <c r="A34" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="G34" t="s">
         <v>74</v>
-      </c>
-      <c r="G34" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="13.2">
       <c r="A35" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="G35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="13.2">
       <c r="A36" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>79</v>
+        <v>446</v>
       </c>
       <c r="G36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="13.2">
       <c r="A37" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="G37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="13.2">
       <c r="A38" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>83</v>
-      </c>
       <c r="G38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="13.2">
@@ -9415,38 +9581,38 @@
     </row>
     <row r="40" spans="1:7" ht="13.2">
       <c r="A40" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" t="s">
         <v>84</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="G40" t="s">
         <v>86</v>
-      </c>
-      <c r="G40" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="13.2">
       <c r="A41" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="G41" t="s">
         <v>89</v>
-      </c>
-      <c r="G41" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="13.2">
       <c r="A42" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>92</v>
-      </c>
       <c r="G42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -9454,38 +9620,38 @@
     </row>
     <row r="44" spans="1:7" ht="13.2">
       <c r="A44" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" t="s">
         <v>93</v>
       </c>
-      <c r="C44" t="s">
-        <v>94</v>
-      </c>
       <c r="D44" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="G44" t="s">
         <v>95</v>
-      </c>
-      <c r="G44" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="13.2">
       <c r="A45" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="G45" t="s">
         <v>98</v>
-      </c>
-      <c r="G45" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="13.2">
       <c r="A46" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="G46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -9493,19 +9659,19 @@
     </row>
     <row r="49" spans="1:8" ht="13.2">
       <c r="A49" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" t="s">
         <v>102</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>103</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="G49" t="s">
         <v>105</v>
-      </c>
-      <c r="G49" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -9513,417 +9679,418 @@
     </row>
     <row r="52" spans="1:8" ht="13.2">
       <c r="A52" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s">
         <v>107</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>108</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="G52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="13.2">
       <c r="A53" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="G53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="13.2">
       <c r="A54" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="G54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="13.2">
       <c r="A55" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="G55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="26.4">
       <c r="A56" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="G56" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="13.2">
       <c r="A57" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="G57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="13.2">
       <c r="A58" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D58" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D58" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="G58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="13.2">
       <c r="A59" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D59" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="D59" s="9" t="s">
+      <c r="G59" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="13.2">
+      <c r="A60" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="G60" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="13.2">
+      <c r="A61" s="6"/>
+      <c r="D61" s="9"/>
+    </row>
+    <row r="62" spans="1:8" s="15" customFormat="1" ht="13.2">
+      <c r="A62" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="G59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="D60"/>
-    </row>
-    <row r="61" spans="1:8" s="15" customFormat="1" ht="13.2">
-      <c r="A61" s="14" t="s">
+      <c r="C62" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="D62" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="H62" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="H61" s="16" t="s">
+    </row>
+    <row r="63" spans="1:8" ht="13.2">
+      <c r="A63" s="6" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="13.2">
-      <c r="A62" s="6" t="s">
+      <c r="D63" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="D62" s="6" t="s">
+    </row>
+    <row r="64" spans="1:8" s="18" customFormat="1" ht="13.2">
+      <c r="A64" s="17" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" s="18" customFormat="1" ht="13.2">
-      <c r="A63" s="17" t="s">
+      <c r="D64" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="D63" s="17" t="s">
+      <c r="H64" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="H63" s="19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="D64"/>
-    </row>
-    <row r="65" spans="1:7" ht="13.2">
-      <c r="A65" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B65" t="s">
-        <v>135</v>
-      </c>
-      <c r="C65" t="s">
-        <v>136</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G65" t="s">
-        <v>138</v>
-      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="D65"/>
     </row>
     <row r="66" spans="1:7" ht="13.2">
       <c r="A66" s="6" t="s">
-        <v>139</v>
+        <v>133</v>
+      </c>
+      <c r="B66" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" t="s">
+        <v>135</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="13.2">
       <c r="A67" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="13.2">
       <c r="A68" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="13.2">
       <c r="A69" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G69" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="13.2">
       <c r="A70" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="13.2">
+      <c r="A71" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G70" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="D71"/>
-    </row>
-    <row r="72" spans="1:7" ht="13.2">
-      <c r="A72" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C72" t="s">
-        <v>150</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="G72" s="20" t="s">
-        <v>152</v>
-      </c>
+      <c r="G71" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="D72"/>
     </row>
     <row r="73" spans="1:7" ht="13.2">
       <c r="A73" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
+      </c>
+      <c r="C73" t="s">
+        <v>149</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G73" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="13.2">
       <c r="A74" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G74" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="13.2">
       <c r="A75" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G75" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="13.2">
       <c r="A76" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G76" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="13.2">
       <c r="A77" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G77" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="13.2">
       <c r="A78" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G78" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="13.2">
       <c r="A79" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G79" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="13.2">
       <c r="A80" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="G80" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="13.2">
       <c r="A81" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G81" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="13.2">
       <c r="A82" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G82" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="13.2">
+      <c r="A83" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D83" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="D82" s="9" t="s">
+      <c r="G83" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="D84"/>
+    </row>
+    <row r="86" spans="1:7" s="38" customFormat="1" ht="13.2">
+      <c r="A86" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="G82" s="20" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="D83"/>
-    </row>
-    <row r="85" spans="1:7" ht="13.2">
-      <c r="A85" s="6" t="s">
+      <c r="B86" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C86" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="C85" t="s">
-        <v>27</v>
-      </c>
-      <c r="D85" s="8" t="s">
+      <c r="G86" s="38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="38" customFormat="1" ht="13.2">
+      <c r="A87" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="G85" t="s">
+      <c r="D87" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="G87" s="38" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="13.2">
-      <c r="A86" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="D86" s="8" t="s">
+    <row r="88" spans="1:7" s="38" customFormat="1" ht="13.2">
+      <c r="A88" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="G86" t="s">
+      <c r="D88" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="G88" s="38" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="13.2">
-      <c r="A87" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D87" s="8" t="s">
+    <row r="89" spans="1:7" s="38" customFormat="1" ht="13.2">
+      <c r="A89" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="G87" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="13.2">
-      <c r="A88" s="6" t="s">
+      <c r="D89" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="D88" s="8" t="s">
+    </row>
+    <row r="90" spans="1:7" s="38" customFormat="1" ht="13.2">
+      <c r="A90" s="37" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="13.2">
-      <c r="A89" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D89" s="8" t="s">
+      <c r="D90" s="39" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
-      <c r="D90"/>
-    </row>
-    <row r="91" spans="1:7" ht="13.2">
-      <c r="A91" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C91" t="s">
-        <v>37</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G91" t="s">
-        <v>29</v>
-      </c>
+    <row r="91" spans="1:7">
+      <c r="D91"/>
     </row>
     <row r="92" spans="1:7" ht="13.2">
       <c r="A92" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
+      </c>
+      <c r="C92" t="s">
+        <v>37</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G92" t="s">
         <v>29</v>
@@ -9931,10 +10098,10 @@
     </row>
     <row r="93" spans="1:7" ht="13.2">
       <c r="A93" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G93" t="s">
         <v>29</v>
@@ -9942,10 +10109,10 @@
     </row>
     <row r="94" spans="1:7" ht="13.2">
       <c r="A94" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="D94" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="G94" t="s">
         <v>29</v>
@@ -9953,10 +10120,10 @@
     </row>
     <row r="95" spans="1:7" ht="13.2">
       <c r="A95" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G95" t="s">
         <v>29</v>
@@ -9964,24 +10131,29 @@
     </row>
     <row r="96" spans="1:7" ht="13.2">
       <c r="A96" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G96" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="13.2">
+      <c r="A97" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D97" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="D96" s="9" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="13.2">
-      <c r="D97"/>
-      <c r="G97" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="13.2">
       <c r="A98" s="6" t="s">
-        <v>195</v>
+        <v>450</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>196</v>
+        <v>451</v>
       </c>
       <c r="G98" t="s">
         <v>29</v>
@@ -9989,10 +10161,10 @@
     </row>
     <row r="99" spans="1:8" ht="13.2">
       <c r="A99" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="D99" s="9" t="s">
-        <v>198</v>
+        <v>194</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="G99" t="s">
         <v>29</v>
@@ -10000,32 +10172,32 @@
     </row>
     <row r="100" spans="1:8" ht="13.2">
       <c r="A100" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="G100" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="52.8">
+    <row r="101" spans="1:8" ht="13.2">
       <c r="A101" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G101" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="13.2">
+    <row r="102" spans="1:8" ht="52.8">
       <c r="A102" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G102" t="s">
         <v>29</v>
@@ -10033,10 +10205,10 @@
     </row>
     <row r="103" spans="1:8" ht="13.2">
       <c r="A103" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G103" t="s">
         <v>29</v>
@@ -10044,76 +10216,89 @@
     </row>
     <row r="104" spans="1:8" ht="13.2">
       <c r="A104" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>204</v>
+        <v>64</v>
+      </c>
+      <c r="G104" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="13.2">
       <c r="A105" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>70</v>
+        <v>203</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="13.2">
-      <c r="D106" s="8"/>
+      <c r="A106" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="107" spans="1:8" ht="13.2">
       <c r="A107" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>207</v>
+        <v>452</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="13.2">
       <c r="A108" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="13.2">
       <c r="A109" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="13.2">
+      <c r="A110" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D110" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="D109" s="8" t="s">
+    </row>
+    <row r="111" spans="1:8" s="22" customFormat="1" ht="13.2">
+      <c r="A111" s="21" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" s="22" customFormat="1" ht="13.2">
-      <c r="A110" s="21" t="s">
+      <c r="D111" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="D110" s="23" t="s">
+      <c r="H111" s="24" t="s">
         <v>213</v>
-      </c>
-      <c r="H110" s="24" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="13.2">
-      <c r="A111" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D111" s="8" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="13.2">
       <c r="A112" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="13.2">
+      <c r="A113" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D113" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="D112" s="8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="13.2">
-      <c r="D113" s="8"/>
     </row>
     <row r="114" spans="1:7" ht="13.2">
       <c r="D114" s="8"/>
@@ -10124,104 +10309,107 @@
     <row r="116" spans="1:7" ht="13.2">
       <c r="D116" s="8"/>
     </row>
-    <row r="117" spans="1:7">
-      <c r="D117"/>
-    </row>
-    <row r="118" spans="1:7" ht="13.2">
-      <c r="A118" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="C118" t="s">
-        <v>85</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G118" t="s">
-        <v>87</v>
-      </c>
+    <row r="117" spans="1:7" ht="13.2">
+      <c r="D117" s="8"/>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="D118"/>
     </row>
     <row r="119" spans="1:7" ht="13.2">
       <c r="A119" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
+      </c>
+      <c r="C119" t="s">
+        <v>84</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>221</v>
+        <v>85</v>
+      </c>
+      <c r="G119" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="13.2">
       <c r="A120" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G120" t="s">
-        <v>90</v>
+        <v>220</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="13.2">
       <c r="A121" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G121" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7">
-      <c r="D122"/>
-    </row>
-    <row r="123" spans="1:7" ht="13.2">
-      <c r="A123" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C123" t="s">
-        <v>94</v>
-      </c>
-      <c r="D123" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="G123" t="s">
-        <v>96</v>
-      </c>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="13.2">
+      <c r="A122" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G122" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="D123"/>
     </row>
     <row r="124" spans="1:7" ht="13.2">
       <c r="A124" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="C124" t="s">
+        <v>93</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>226</v>
+        <v>94</v>
+      </c>
+      <c r="G124" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="13.2">
       <c r="A125" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G125" t="s">
-        <v>99</v>
+        <v>225</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="13.2">
       <c r="A126" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G126" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="13.2">
+      <c r="A127" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G127" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12页 &amp;P</oddFooter>
@@ -10233,8 +10421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -10276,23 +10464,23 @@
     </row>
     <row r="3" spans="1:7" ht="176.25" customHeight="1">
       <c r="A3" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>229</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>230</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>232</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.5" customHeight="1">
@@ -10302,10 +10490,10 @@
     </row>
     <row r="8" spans="1:7" ht="13.2">
       <c r="A8" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8" t="s">
         <v>234</v>
-      </c>
-      <c r="B8" t="s">
-        <v>235</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -10316,7 +10504,7 @@
     </row>
     <row r="9" spans="1:7" ht="13.2">
       <c r="A9" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -10324,7 +10512,7 @@
     </row>
     <row r="10" spans="1:7" ht="13.2">
       <c r="A10" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>23</v>
@@ -10332,7 +10520,7 @@
     </row>
     <row r="11" spans="1:7" ht="13.2">
       <c r="A11" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>25</v>
@@ -10340,10 +10528,10 @@
     </row>
     <row r="12" spans="1:7" ht="13.2">
       <c r="A12" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>239</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -10351,42 +10539,42 @@
     </row>
     <row r="14" spans="1:7" ht="13.2">
       <c r="A14" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="13.2">
       <c r="A15" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="13.2">
       <c r="A16" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13.2">
       <c r="A17" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.2">
       <c r="A18" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>35</v>
@@ -10397,53 +10585,53 @@
     </row>
     <row r="20" spans="1:4" ht="13.2">
       <c r="A20" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C20" t="s">
         <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13.2">
       <c r="A21" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="D21" t="s">
         <v>249</v>
-      </c>
-      <c r="D21" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13.2">
       <c r="A22" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>251</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13.2">
       <c r="A23" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D23" s="20" t="s">
         <v>253</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.2">
       <c r="A24" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="D24" s="20" t="s">
         <v>255</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13.2">
       <c r="A25" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>257</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -10451,298 +10639,298 @@
     </row>
     <row r="27" spans="1:4" ht="13.2">
       <c r="A27" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D27" t="s">
         <v>259</v>
-      </c>
-      <c r="D27" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.2">
       <c r="A28" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D28" t="s">
         <v>261</v>
-      </c>
-      <c r="D28" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13.2">
       <c r="A29" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>263</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.2">
       <c r="A30" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>265</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13.2">
       <c r="A31" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>267</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13.2">
       <c r="A32" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13.2">
       <c r="A33" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="D33" s="20" t="s">
         <v>271</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13.2">
       <c r="A35" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13.2">
       <c r="A36" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="13.2">
       <c r="A37" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="13.2">
       <c r="A38" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4">
       <c r="A39" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="13.2">
       <c r="A40" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>283</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="13.2">
       <c r="A41" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D41" s="9" t="s">
         <v>285</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="13.2">
       <c r="A42" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="13.2">
       <c r="A43" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="13.2">
       <c r="A44" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="13.2">
       <c r="A45" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D45" s="9" t="s">
         <v>293</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="13.2">
       <c r="A47" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D47" t="s">
         <v>295</v>
-      </c>
-      <c r="D47" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="13.2">
       <c r="A48" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="D48" t="s">
         <v>297</v>
-      </c>
-      <c r="D48" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="13.2">
       <c r="A49" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D49" s="20" t="s">
         <v>299</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="13.2">
       <c r="A50" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="D50" s="20" t="s">
         <v>301</v>
-      </c>
-      <c r="D50" s="20" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="13.2">
       <c r="A51" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="D51" s="20" t="s">
         <v>303</v>
-      </c>
-      <c r="D51" s="20" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="13.2">
       <c r="A52" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D52" s="20" t="s">
         <v>305</v>
-      </c>
-      <c r="D52" s="20" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="13.2">
       <c r="A53" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="D53" s="20" t="s">
         <v>307</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="13.2">
       <c r="A55" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D55" t="s">
         <v>309</v>
-      </c>
-      <c r="D55" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="13.2">
       <c r="A56" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D56" t="s">
         <v>311</v>
-      </c>
-      <c r="D56" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="13.2">
       <c r="A57" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="D57" s="20" t="s">
         <v>313</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="13.2">
       <c r="A58" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="D58" s="20" t="s">
         <v>315</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="13.2">
       <c r="A59" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D59" s="20" t="s">
         <v>317</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="13.2">
       <c r="A60" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>319</v>
-      </c>
-      <c r="D60" s="20" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="13.2">
       <c r="A61" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>321</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="13.2">
       <c r="A63" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="D63" t="s">
         <v>323</v>
-      </c>
-      <c r="D63" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="13.2">
       <c r="A64" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="D64" t="s">
         <v>325</v>
-      </c>
-      <c r="D64" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="13.2">
       <c r="A65" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="D65" s="20" t="s">
         <v>327</v>
-      </c>
-      <c r="D65" s="20" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="13.2">
       <c r="A66" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D66" s="20" t="s">
         <v>329</v>
-      </c>
-      <c r="D66" s="20" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="13.2">
       <c r="A67" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D67" s="20" t="s">
         <v>331</v>
-      </c>
-      <c r="D67" s="20" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -10750,50 +10938,50 @@
     </row>
     <row r="69" spans="1:4" ht="13.2">
       <c r="A69" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D69" s="20" t="s">
         <v>333</v>
-      </c>
-      <c r="D69" s="20" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="13.2">
       <c r="A70" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="D70" t="s">
         <v>335</v>
-      </c>
-      <c r="D70" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="13.2">
       <c r="A71" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="D71" s="20" t="s">
         <v>337</v>
-      </c>
-      <c r="D71" s="20" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="13.2">
       <c r="A72" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="D72" s="20" t="s">
         <v>339</v>
-      </c>
-      <c r="D72" s="20" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="13.2">
       <c r="A73" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="D73" s="20" t="s">
         <v>341</v>
-      </c>
-      <c r="D73" s="20" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="13.2">
       <c r="A74" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="D74" s="20" t="s">
         <v>343</v>
-      </c>
-      <c r="D74" s="20" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -10801,178 +10989,178 @@
     </row>
     <row r="76" spans="1:4" ht="13.2">
       <c r="A76" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="D76" s="20" t="s">
         <v>345</v>
-      </c>
-      <c r="D76" s="20" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="13.2">
       <c r="A77" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D77" t="s">
         <v>347</v>
-      </c>
-      <c r="D77" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="13.2">
       <c r="A78" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="D78" s="20" t="s">
         <v>349</v>
-      </c>
-      <c r="D78" s="20" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="13.2">
       <c r="A79" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D79" s="20" t="s">
         <v>351</v>
-      </c>
-      <c r="D79" s="20" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="13.2">
       <c r="A80" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="D80" s="20" t="s">
         <v>353</v>
-      </c>
-      <c r="D80" s="20" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="13.2">
       <c r="A81" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="D81" s="20" t="s">
         <v>355</v>
-      </c>
-      <c r="D81" s="20" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="13.2">
       <c r="A83" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="C83" t="s">
         <v>357</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" s="20" t="s">
         <v>358</v>
-      </c>
-      <c r="D83" s="20" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="13.2">
       <c r="A84" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="D84" t="s">
         <v>360</v>
-      </c>
-      <c r="D84" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="13.2">
       <c r="A85" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="D85" s="20" t="s">
         <v>362</v>
-      </c>
-      <c r="D85" s="20" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="13.2">
       <c r="A86" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="D86" s="20" t="s">
         <v>364</v>
-      </c>
-      <c r="D86" s="20" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="13.2">
       <c r="A87" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="D87" s="20" t="s">
         <v>366</v>
-      </c>
-      <c r="D87" s="20" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="13.2">
       <c r="A88" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D88" s="20" t="s">
         <v>368</v>
-      </c>
-      <c r="D88" s="20" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="13.2">
       <c r="A89" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="D89" s="20" t="s">
         <v>370</v>
-      </c>
-      <c r="D89" s="20" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="13.2">
       <c r="A91" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C91" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D91" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G91" t="s">
         <v>89</v>
-      </c>
-      <c r="G91" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="13.2">
       <c r="A92" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="13.2">
       <c r="A94" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C94" t="s">
+        <v>93</v>
+      </c>
+      <c r="D94" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D94" s="8" t="s">
+      <c r="G94" t="s">
         <v>95</v>
-      </c>
-      <c r="G94" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="13.2">
       <c r="A95" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="13.2">
       <c r="A96" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D96" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G96" t="s">
         <v>98</v>
-      </c>
-      <c r="G96" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="13.2">
       <c r="A97" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G97" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -10990,7 +11178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I44" sqref="I44:I45"/>
     </sheetView>
   </sheetViews>
@@ -11003,86 +11191,86 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.4">
       <c r="A1" s="31" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1">
       <c r="A2" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>378</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>379</v>
-      </c>
       <c r="C2" s="27" t="s">
+        <v>417</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>418</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>419</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
       <c r="G2" s="27" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H2" s="27"/>
       <c r="I2" s="30" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="J2" s="29"/>
       <c r="K2" s="25"/>
     </row>
     <row r="3" spans="1:11" ht="14.4">
       <c r="A3" s="27" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="43.2">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.4">
       <c r="A4" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
       <c r="D4" s="28" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
       <c r="I4" s="27" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="43.2">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.4">
       <c r="A5" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
       <c r="D5" s="28" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
       <c r="I5" s="27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.4">
@@ -11098,484 +11286,484 @@
     </row>
     <row r="7" spans="1:11" ht="14.4">
       <c r="A7" s="27" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="27" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.4">
       <c r="A8" s="30" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="35" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E8" s="34"/>
       <c r="F8" s="34"/>
       <c r="G8" s="34" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H8" s="34"/>
       <c r="I8" s="33" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="34" customFormat="1" ht="14.4">
       <c r="A9" s="30" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I9" s="33" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="14.4">
       <c r="A10" s="30" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
       <c r="D10" s="35" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
       <c r="G10" s="34" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H10" s="34"/>
       <c r="I10" s="34" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="14.4">
       <c r="A12" s="30" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="34" t="s">
+        <v>434</v>
+      </c>
+      <c r="D12" s="35" t="s">
         <v>435</v>
-      </c>
-      <c r="D12" s="35" t="s">
-        <v>436</v>
       </c>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
       <c r="G12" s="34" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H12" s="34"/>
       <c r="I12" s="36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="14.4">
       <c r="A13" s="30" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
       <c r="D13" s="35" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E13" s="34"/>
       <c r="F13" s="34"/>
       <c r="G13" s="34" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H13" s="34"/>
       <c r="I13" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="14.4">
       <c r="A14" s="30" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B14" s="34"/>
       <c r="C14" s="34"/>
       <c r="D14" s="35" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E14" s="34"/>
       <c r="F14" s="34"/>
       <c r="G14" s="34" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H14" s="34"/>
       <c r="I14" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.4">
       <c r="A15" s="30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E15" s="34"/>
       <c r="F15" s="34"/>
       <c r="G15" s="34" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H15" s="34"/>
       <c r="I15" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="28.8">
       <c r="A16" s="30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E16" s="34"/>
       <c r="F16" s="34"/>
       <c r="G16" s="34" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H16" s="34"/>
       <c r="I16" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="14.4">
       <c r="A17" s="30" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
       <c r="D17" s="35" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E17" s="34"/>
       <c r="F17" s="34"/>
       <c r="G17" s="34" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H17" s="34"/>
       <c r="I17" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.4">
       <c r="A18" s="32" t="s">
+        <v>392</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>394</v>
-      </c>
       <c r="G18" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I18" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="14.4">
       <c r="A19" s="32" t="s">
+        <v>394</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>396</v>
-      </c>
       <c r="G19" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="13.2">
       <c r="A20" s="32" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="14.4">
       <c r="A21" s="32" t="s">
+        <v>397</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>399</v>
-      </c>
       <c r="G21" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I21" s="36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="14.4">
       <c r="A22" s="32" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I22" s="36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="14.4">
       <c r="A23" s="32" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="52.8">
       <c r="A24" s="32" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I24" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="14.4">
       <c r="A25" s="32" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I25" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="14.4">
       <c r="A26" s="32" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="14.4">
       <c r="A27" s="32" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I27" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="14.4">
       <c r="A29" s="32" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G29" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I29" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="14.4">
       <c r="A30" s="32" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D30" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="G30" s="31" t="s">
-        <v>75</v>
-      </c>
       <c r="I30" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="14.4">
       <c r="A31" s="32" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G31" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I31" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="14.4">
       <c r="A32" s="32" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G32" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I32" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="14.4">
       <c r="A33" s="32" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G33" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I33" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="14.4">
       <c r="A34" s="32" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G34" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I34" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="14.4">
       <c r="I35" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="14.4">
       <c r="A36" s="32" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C36" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="G36" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="G36" s="31" t="s">
-        <v>87</v>
-      </c>
       <c r="I36" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="14.4">
       <c r="A37" s="32" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D37" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="G37" s="31" t="s">
-        <v>90</v>
-      </c>
       <c r="I37" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="14.4">
       <c r="A38" s="32" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G38" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I38" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="14.4">
       <c r="A40" s="32" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C40" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="G40" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="G40" s="31" t="s">
-        <v>96</v>
-      </c>
       <c r="I40" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="14.4">
       <c r="A41" s="32" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I41" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="14.4">
       <c r="A42" s="32" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G42" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I42" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add TC1084 to TC1088
</commit_message>
<xml_diff>
--- a/testcase/testcase.xlsx
+++ b/testcase/testcase.xlsx
@@ -8640,7 +8640,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8679,12 +8679,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -8745,7 +8739,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -8805,15 +8799,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="好" xfId="2" builtinId="26"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="2" builtinId="26"/>
     <cellStyle name="计算" xfId="1" builtinId="22"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9176,8 +9165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -10024,58 +10013,58 @@
     <row r="84" spans="1:7">
       <c r="D84"/>
     </row>
-    <row r="86" spans="1:7" s="38" customFormat="1" ht="13.2">
-      <c r="A86" s="37" t="s">
+    <row r="86" spans="1:7" ht="13.2">
+      <c r="A86" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="B86" s="38" t="s">
+      <c r="B86" t="s">
         <v>173</v>
       </c>
-      <c r="C86" s="38" t="s">
+      <c r="C86" t="s">
         <v>27</v>
       </c>
-      <c r="D86" s="39" t="s">
+      <c r="D86" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G86" s="38" t="s">
+      <c r="G86" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="38" customFormat="1" ht="13.2">
-      <c r="A87" s="37" t="s">
+    <row r="87" spans="1:7" ht="13.2">
+      <c r="A87" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="D87" s="39" t="s">
+      <c r="D87" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G87" s="38" t="s">
+      <c r="G87" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="1:7" s="38" customFormat="1" ht="13.2">
-      <c r="A88" s="37" t="s">
+    <row r="88" spans="1:7" ht="13.2">
+      <c r="A88" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="D88" s="39" t="s">
+      <c r="D88" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G88" s="38" t="s">
+      <c r="G88" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:7" s="38" customFormat="1" ht="13.2">
-      <c r="A89" s="37" t="s">
+    <row r="89" spans="1:7" ht="13.2">
+      <c r="A89" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D89" s="39" t="s">
+      <c r="D89" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="38" customFormat="1" ht="13.2">
-      <c r="A90" s="37" t="s">
+    <row r="90" spans="1:7" ht="13.2">
+      <c r="A90" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D90" s="39" t="s">
+      <c r="D90" s="1" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add one wancoin test case
</commit_message>
<xml_diff>
--- a/testcase/testcase.xlsx
+++ b/testcase/testcase.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="457">
   <si>
     <t>序号</t>
   </si>
@@ -8566,6 +8566,18 @@
       </rPr>
       <t>填写空字符串</t>
     </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC1127</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>从同一个OTA地址提取两次</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一次提取成功，第二次提取失败</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -9163,10 +9175,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H127"/>
+  <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B104" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G130" sqref="G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -10395,6 +10410,17 @@
         <v>98</v>
       </c>
     </row>
+    <row r="129" spans="1:7" ht="13.2">
+      <c r="A129" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="G129" t="s">
+        <v>456</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -10411,7 +10437,7 @@
   <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>

</xml_diff>